<commit_message>
Add range and sheet options for loading data from Excel
Used ANTLR for parsing the Excel range syntax. Currently offer 3 forms:

 1. 'A1:B2' - Complete Range
 2. 'A1'    - Just the start cell
 3. '1:A:C' - Start row with columns specified (like excelchop)

Only 1 and 2 are implemented.

This also required being more explicit about the working directory
while evaluating expressions, since the path can be relative, and it's
important to know what location the file is in.

This also added an extension method for sanitizing identifiers supplied
by the user. This is used when parsing the headers of data.
</commit_message>
<xml_diff>
--- a/test/test_files/Excel/load_test.xlsx
+++ b/test/test_files/Excel/load_test.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23808"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3244018C-1C2B-46F0-916B-A026C5365FEF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5105975C-32BB-484A-B6BE-666E0612564E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="New Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="8">
   <si>
     <t>name</t>
   </si>
@@ -41,6 +42,15 @@
   </si>
   <si>
     <t>Zone 2</t>
+  </si>
+  <si>
+    <t>Other stuff</t>
+  </si>
+  <si>
+    <t>Zone 3</t>
+  </si>
+  <si>
+    <t>Zone 4</t>
   </si>
 </sst>
 </file>
@@ -394,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -436,4 +446,60 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75E4F0B4-F80E-4D72-8CEE-BAD4BB46099D}">
+  <dimension ref="A1:K8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="I6" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" t="s">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="I7" t="s">
+        <v>6</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="I8" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8">
+        <v>5</v>
+      </c>
+      <c r="K8">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>